<commit_message>
hazlo en el documentos ese
</commit_message>
<xml_diff>
--- a/pl2 tabla.xlsx
+++ b/pl2 tabla.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Entidad/Relacion</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Dominio</t>
   </si>
   <si>
-    <t>Restriccion</t>
+    <t>Restricción</t>
   </si>
   <si>
     <t>PK/CK/Discriminante</t>
@@ -34,28 +34,52 @@
     <t>Año</t>
   </si>
   <si>
+    <t>INT</t>
+  </si>
+  <si>
     <t>PK</t>
   </si>
   <si>
     <t>Titulo</t>
   </si>
   <si>
+    <t>CHAR(40)</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
     <t>Duracion</t>
   </si>
   <si>
+    <t>Float</t>
+  </si>
+  <si>
     <t>Idioma</t>
   </si>
   <si>
+    <t>CHAR(10)</t>
+  </si>
+  <si>
     <t>Calificacion</t>
   </si>
   <si>
+    <t>[1]</t>
+  </si>
+  <si>
     <t>Generos</t>
   </si>
   <si>
     <t>Personal</t>
   </si>
   <si>
-    <t>DNI?</t>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>CHAR(8)</t>
+  </si>
+  <si>
+    <t>[2]</t>
   </si>
   <si>
     <t>Nombre</t>
@@ -64,6 +88,9 @@
     <t>Año de nacimiento</t>
   </si>
   <si>
+    <t>int</t>
+  </si>
+  <si>
     <t>Nacionalidad</t>
   </si>
   <si>
@@ -76,7 +103,7 @@
     <t>Criticas</t>
   </si>
   <si>
-    <t>Id¿</t>
+    <t>Id</t>
   </si>
   <si>
     <t>Critico</t>
@@ -88,6 +115,9 @@
     <t>Texto</t>
   </si>
   <si>
+    <t>CHAR(400)</t>
+  </si>
+  <si>
     <t>Caratulas</t>
   </si>
   <si>
@@ -97,21 +127,36 @@
     <t>Tipo</t>
   </si>
   <si>
+    <t>-NO SE Q ES-</t>
+  </si>
+  <si>
     <t>PaginaWeb</t>
   </si>
   <si>
     <t>Url</t>
   </si>
   <si>
+    <t>CHAR(100)</t>
+  </si>
+  <si>
+    <t>alojadas</t>
+  </si>
+  <si>
+    <t>1,n</t>
+  </si>
+  <si>
     <t>Alojadas</t>
   </si>
   <si>
-    <t>1,n</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>tiene</t>
+  </si>
+  <si>
     <t>Tiene</t>
   </si>
   <si>
@@ -121,7 +166,19 @@
     <t>Papel</t>
   </si>
   <si>
+    <t>CHAR(20)</t>
+  </si>
+  <si>
     <t>Dirige</t>
+  </si>
+  <si>
+    <t>[1] Es un entero  dentro del rango [0-10]</t>
+  </si>
+  <si>
+    <t>[2]  Dividimos el número completo del DNI entre 23, sin sacar decimales. Utilizamos el resto de la división para calcular la letra.</t>
+  </si>
+  <si>
+    <t>[3] Solo letras y espacio entre palabras, primera de cada palabra en mayúsculas</t>
   </si>
 </sst>
 </file>
@@ -132,12 +189,12 @@
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
       <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -145,7 +202,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +211,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF63D297"/>
+        <bgColor rgb="FF63D297"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7F9EF"/>
+        <bgColor rgb="FFE7F9EF"/>
       </patternFill>
     </fill>
   </fills>
@@ -165,21 +234,43 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -192,52 +283,52 @@
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1A1A1A"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="EEF1F1"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1A1A1A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="EEF1F1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="1A9988"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="2D729D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="1F3E78"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="EB5600"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="FF99AC"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="FFD4B8"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1F3E78"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1F3E78"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Verdana"/>
+        <a:ea typeface="Verdana"/>
+        <a:cs typeface="Verdana"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Verdana"/>
+        <a:ea typeface="Verdana"/>
+        <a:cs typeface="Verdana"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,11 +480,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.5"/>
-    <col customWidth="1" min="2" max="2" width="15.25"/>
-    <col customWidth="1" min="5" max="5" width="19.75"/>
+    <col customWidth="1" min="1" max="1" width="14.67"/>
+    <col customWidth="1" min="2" max="2" width="13.56"/>
+    <col customWidth="1" min="5" max="5" width="17.56"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -417,193 +508,346 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+    </row>
+    <row r="4">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="1" t="s">
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="1" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="D23" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="7"/>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>31</v>
+      <c r="A28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -614,6 +858,16 @@
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A20"/>
   </mergeCells>
+  <conditionalFormatting sqref="A1:E28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFFFFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>